<commit_message>
Dodana ispravljene verzije kupovine karata
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Kupovina karata.xlsx
+++ b/UseCaseScenarij/Kupovina karata.xlsx
@@ -31,9 +31,6 @@
     <t>Preduvjeti</t>
   </si>
   <si>
-    <t>Korisnik mora imati otvoren račun na Internetu.</t>
-  </si>
-  <si>
     <t>Posljedice – uspješan završetak</t>
   </si>
   <si>
@@ -43,9 +40,6 @@
     <t>Posljedice – neuspješan završetak</t>
   </si>
   <si>
-    <t xml:space="preserve">Korisnik dobiva obavijest  da ne može kupiti željenu kartu i razloge zbog kojih ne može kupiti kartu(nema otvoren račun na Internetu ili nema karata). </t>
-  </si>
-  <si>
     <t>Primarni akteri</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
   </si>
   <si>
     <t>Glavni tok</t>
-  </si>
-  <si>
-    <t>Putnik podnosi zahtjev za kupovinu, bira željenu kartu, plaća preko PayPal-a.</t>
   </si>
   <si>
     <t>Proširenja/Alternative</t>
@@ -264,8 +255,17 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>8.</t>
+    <t>Alternativni tok: Neuspješna validacija.</t>
+  </si>
+  <si>
+    <t>Preduslov: Nije zadovoljen korak 5.</t>
+  </si>
+  <si>
+    <t>Tok događaja:</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
     </r>
     <r>
       <rPr>
@@ -286,21 +286,12 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Validacija unesenih podataka.</t>
-    </r>
-  </si>
-  <si>
-    <t>Alternativni tok: Neuspješna validacija.</t>
-  </si>
-  <si>
-    <t>Preduslov: Nije zadovoljen korak 5.</t>
-  </si>
-  <si>
-    <t>Tok događaja:</t>
-  </si>
-  <si>
-    <r>
-      <t>1.</t>
+      <t>Narudžba ne prolazi, jer odabrana karta nije dostupna.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
     </r>
     <r>
       <rPr>
@@ -321,12 +312,12 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Narudžba ne prolazi, jer odabrana karta nije dostupna.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2.</t>
+      <t>Obavještavanje korisnika.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
     </r>
     <r>
       <rPr>
@@ -347,12 +338,30 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Obavještavanje korisnika.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3.</t>
+      <t>Vraćanje na korak 4.</t>
+    </r>
+  </si>
+  <si>
+    <t>10.   Izvještavanje da je transakcija prihvaćena.</t>
+  </si>
+  <si>
+    <t>11.   Odlazak kupca po kartu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korisnik dobiva obavijest  da ne može kupiti željenu kartu i razloge zbog kojih ne može kupiti kartu. </t>
+  </si>
+  <si>
+    <t>Putnik podnosi zahtjev za kupovinu, bira željenu kartu, uplaćuje novac na Grasov račun</t>
+  </si>
+  <si>
+    <t>Korisnik mora uplatiti iznos na Grasov račun</t>
+  </si>
+  <si>
+    <t>9.  Prosljeđivanje transakcije Sistemu za autorizaciju računa.</t>
+  </si>
+  <si>
+    <r>
+      <t>8.</t>
     </r>
     <r>
       <rPr>
@@ -362,7 +371,7 @@
         <family val="1"/>
         <charset val="238"/>
       </rPr>
-      <t xml:space="preserve">       </t>
+      <t>      </t>
     </r>
     <r>
       <rPr>
@@ -373,29 +382,28 @@
         <charset val="238"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Vraćanje na korak 4.</t>
-    </r>
-  </si>
-  <si>
-    <t>9.       Prosljeđivanje transakcije Sistemu za autorizaciju računa.</t>
-  </si>
-  <si>
-    <t>10.   Izvještavanje da je transakcija prihvaćena.</t>
-  </si>
-  <si>
-    <t>11.   Odlazak kupca po kartu</t>
+      <t>Validacija unesenih podataka.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -510,59 +518,62 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -872,14 +883,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -904,55 +915,55 @@
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="4" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="90.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="B8" s="4" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -969,7 +980,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
@@ -983,63 +994,63 @@
     </row>
     <row r="18" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" ht="128.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" ht="93.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="10"/>
       <c r="B22" s="9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" ht="88.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="9" t="s">
-        <v>29</v>
+        <v>25</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="C23" s="8"/>
     </row>
     <row r="24" spans="1:3" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1049,7 +1060,7 @@
     </row>
     <row r="26" spans="1:3" ht="56.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="14" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -1062,17 +1073,17 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1080,32 +1091,32 @@
     </row>
     <row r="33" spans="1:3" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="12" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:3" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="12" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:3" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>

</xml_diff>